<commit_message>
Reviewed and added new xpath ,included window handling,enhanced the base class usage,included parameters and group concept of testng
</commit_message>
<xml_diff>
--- a/src/main/resources/HDFCCustomerLoginData.xlsx
+++ b/src/main/resources/HDFCCustomerLoginData.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9A5CF474-0054-4E81-BE7C-5F542EF037CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Repo\selenium-test\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99452A39-0A20-4A9A-B759-58D90694E5D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21660" windowHeight="16500" xr2:uid="{0A13048D-F178-4A2F-B12A-9BFF3CC31F39}"/>
+    <workbookView xWindow="18980" yWindow="0" windowWidth="19420" windowHeight="10400" xr2:uid="{0A13048D-F178-4A2F-B12A-9BFF3CC31F39}"/>
   </bookViews>
   <sheets>
     <sheet name="HDFCCustomerLoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Password</t>
   </si>
@@ -443,7 +448,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,48 +466,98 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
+      <c r="A4" s="2">
+        <v>121212</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4334534543</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>121212</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4334534543</v>
+        <v>23123213</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>23123213</v>
-      </c>
+      <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{12550011-4598-4FD0-90A2-7E855D6E7747}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD309628-70ED-4216-85D4-F087CC3A57F9}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>121212</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4334534543</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>23123213</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>